<commit_message>
add writeup, presentation files, and project info
</commit_message>
<xml_diff>
--- a/data/sources/states.xlsx
+++ b/data/sources/states.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsmith/Documents/__Archivus/CU/BS_CSPB/classes/CSPB3287/PROJECT/state-energy-scout/data/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34402B40-4E5D-5D42-8B02-14907B93A3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81CAD9E-6A57-0144-9F96-932DFF5D6ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="2860" windowWidth="27240" windowHeight="16440" xr2:uid="{DA697190-9C29-4B40-87A7-A2F5645AE278}"/>
   </bookViews>
@@ -714,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F9E74B-AEF3-7049-A0BB-9E91955E8220}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>